<commit_message>
ajout des content et autres modifs
</commit_message>
<xml_diff>
--- a/updates/excels/start_needs.xlsx
+++ b/updates/excels/start_needs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\wakaari\plugins\waka\wcms\updates\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\talktob\plugins\waka\wcms\updates\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A74194-FB91-43B7-881C-115E58DD24C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDF508D-6581-4749-B6DD-3423A3AE678C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{39C5C7BC-0F20-4ABA-B1CF-FB175B7B3F19}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t>name</t>
   </si>
@@ -47,48 +47,15 @@
     <t>description</t>
   </si>
   <si>
-    <t>kpi</t>
-  </si>
-  <si>
     <t>icone</t>
   </si>
   <si>
     <t>Aggrégez vos chiffres de ventes et publiez les sur Word</t>
   </si>
   <si>
-    <t>Envoyez des rapports automatique par email</t>
-  </si>
-  <si>
-    <t>Tenez vos clients informé de l'avancement d'un projet</t>
-  </si>
-  <si>
     <t>Préparez vos réponse aux AO publics</t>
   </si>
   <si>
-    <t>main_image</t>
-  </si>
-  <si>
-    <t>Création d'offres</t>
-  </si>
-  <si>
-    <t>Portail de service BtoB</t>
-  </si>
-  <si>
-    <t>AO publics</t>
-  </si>
-  <si>
-    <t>Campagnes emailing</t>
-  </si>
-  <si>
-    <t>Conception email suivi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Publication de chiffres </t>
-  </si>
-  <si>
-    <t>Suivi automatique de production</t>
-  </si>
-  <si>
     <t>Contrôle d'information</t>
   </si>
   <si>
@@ -108,33 +75,6 @@
   </si>
   <si>
     <t>Controlez votre CRM et tenez informez vos collaborateurs</t>
-  </si>
-  <si>
-    <t>montageLinkedin.jpg</t>
-  </si>
-  <si>
-    <t>portail_service.jpg</t>
-  </si>
-  <si>
-    <t>dc1234.jpg</t>
-  </si>
-  <si>
-    <t>campagne_email2.jpg</t>
-  </si>
-  <si>
-    <t>boite_email_gmail.jpg</t>
-  </si>
-  <si>
-    <t>stat_publish.jpg</t>
-  </si>
-  <si>
-    <t>stats_email.jpg</t>
-  </si>
-  <si>
-    <t>crm_survey.jpg</t>
-  </si>
-  <si>
-    <t>avancement_projet.jpg</t>
   </si>
   <si>
     <t>orem ipsum dolor sit amet, consectetur adipiscing elit. Morbi cursus sit amet nulla at egestas. **Integer** eget elit mauris.  
@@ -156,12 +96,6 @@
 Pellentesque viverra metus in erat semper bibendum. Vivamus auctor venenatis magna eget fermentum.</t>
   </si>
   <si>
-    <t xml:space="preserve">orem ipsum dolor sit amet, consectetur adipiscing elit. Morbi cursus sit amet nulla at egestas. **Integer** eget elit mauris.  
-Proin tristique porta efficitur. Suspendisse potenti. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia Curae; Aliquam semper, ante ut bibendum cursus, tellus urna scelerisque sem, ac viverra tortor tortor nec **libero**.  
-Suspendisse sit amet mauris at augue vestibulum imperdiet id ac tortor. Morbi ac ante euismod, consequat quam vitae, volutpat nisi. Nam aliquet aliquam mi, ut ullamcorper nunc blandit sit amet. Sed ac mattis elit.  
-</t>
-  </si>
-  <si>
     <t>orem ipsum dolor sit amet, consectetur adipiscing elit. Morbi cursus sit amet nulla at egestas. **Intllus urna scelerisque sem, ac viverra tortor tortor nec **libero**.  
 Suspendisse sit amet mauris at augue vestibulum imperdiet id ac tortor. Morbi ac ante euismod, consequat quam vitae, volutpat nisi. Nam aliquet aliquam mi, ut ullamcorper nunc blandit sit amet. Sed ac mattis elit.  
 Integer vestibulum urna at ullamcorper faucibus. Curabitur volutpat justo dui, in mattis est posuere ut. Proin magna sapien, posuere ut dignissim fringilla, ultricies at felis. Aliquam suscipit faucibus magna, ac egestas quam scelerisque id. Sed libero nisi, semper ac ipsum non, eleifend facilisis justo
@@ -176,30 +110,176 @@
    Pellentesque viverra metus in erat semper bibendum. Vivamus auctor venenatis magna eget fermentum.</t>
   </si>
   <si>
-    <t xml:space="preserve">   
-Suspendisse sit amet mauris at augue vestibulum imperdiet id ac tortor. Morbi ac ante euismod, consequat quam vitae, volutpat nisi. Nam aliquet aliquam mi, ut ullamcorper nunc blandit sit amet. Sed ac mattis elit.  
-Integer vestibulum urna at ullamcorper faucibus. Curabitur volutpat justo dui, in mattis est posuere ut. Proin magna sapien, posuere ut dignissim fringilla, ultricies at felis. Aliquam suscipit faucibus magna, ac egestas quam scelerisque id. Sed libero nisi, semper ac ipsum non, eleifend facilisis justo
-* salut
-* toi
-* Encore
-Pellentesque viverra metus in erat semper bibendum. Vivamus auctor venenatis magna eget fermentum.</t>
-  </si>
-  <si>
-    <t>L'offre et la demande désignent respectivement la quantité de produits ou de services que les acteurs sur un marché sont prêts à vendre et/ou à acheter à un prix donné.
-En microéconomie, la théorie de l'équilibre partiel entre l'offre et la demande développée par Alfred Marshall tente de décrire, expliquer, et prédire le prix et la quantité des biens vendus sur les marchés concurrentiels. Le modèle marshalien formalise les théories développées précédemment et est utilisé comme point de départ pour toute une série de modèles et théories économiques et sociales.  
-La théorie de l'offre et de la demande est importante pour certains courants afin de comprendre les mécanismes à l'œuvre dans la décision d'allocation des ressources en économie de marché.</t>
-  </si>
-  <si>
     <t>Pourquoi fideliser : 
 * A court terme : sur des marchés de plus en plus saturés, où la situation concurrentielle se durcit, il apparait que les coûts de prospection de nouveaux clients sont supérieurs aux couts de conservation des clients. Dans cette hypothèse, un opérateur rationnel préfère investir pour conserver les clients qu'il a, plutôt que de tenter de conquérir les clients servis par d'autres fournisseurs. Lesquels en général ne se laisseront pas faire et feront tout pour conserver leurs clients et en particulier les meilleurs. D'où le risque probable de déclenchement d'une guerre des prix, débouchant à terme sur des effets quasi nuls, sinon négatifs : Le partage des volumes reste peu ou prou identique, tandis que le marché global accuse une baisse générale des prix.
 * A moyen, long terme : les études montrent qu'il existe - en longue période - une corrélation entre capacité d'une organisation à fidéliser ses clients (Taux de rétention élevé) et ses résultats concrets (exprimés en part de marché, en rentabilité et en croissance). Les entreprises qui sont en mesure de conserver leur base clientèle et en particulier leurs « bons clients » sont celles qui non seulement résistent le mieux aux dépressions conjoncturelles, mais aussi sont les plus capables de financer leurs projets de développement.</t>
+  </si>
+  <si>
+    <t>solutions</t>
+  </si>
+  <si>
+    <t>absorbtion-saisi, scenarisation-agregation, publication-word, composting</t>
+  </si>
+  <si>
+    <t>portail-service, publication-word, absorbtion-saisi</t>
+  </si>
+  <si>
+    <t>absorbtion-saisi, publication-word</t>
+  </si>
+  <si>
+    <t>Répondre à un appel d'offre public</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scenarisation-agregation, campagne-masse, </t>
+  </si>
+  <si>
+    <t>Fidéliser vos clients</t>
+  </si>
+  <si>
+    <t>absorbtion-saisi, scenarisation-agregation, scenarisation-contenu, contrôle</t>
+  </si>
+  <si>
+    <t>Bilan annuel BU ou Lead Client</t>
+  </si>
+  <si>
+    <t>absorbtion-saisi, scenarisation-agregation, scenarisation-contenu, contrôle, publication-word</t>
+  </si>
+  <si>
+    <t>Envoyer des emails de masse hyperciblé</t>
+  </si>
+  <si>
+    <t>Envoyer des emails de performance hebdomadaire</t>
+  </si>
+  <si>
+    <t>controle, scenarisation-agregation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cloud, </t>
+  </si>
+  <si>
+    <t>Publier de la documentation</t>
+  </si>
+  <si>
+    <t>publication-word, composting</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>Créer une offre</t>
+  </si>
+  <si>
+    <t>faire-une-offre</t>
+  </si>
+  <si>
+    <t>Dans une offre, il y a le coeur de votre proposition, celle où le commercial traduit la problématique du prospect et prouve le bénéfice qu'amènera votre produit ou votre solution. Il y a aussi des contenus qui vont renforcer l'argumentaire : _x000D_
+* Des études de cas client_x000D_
+* Des références_x000D_
+* Le positionnement de votre marque/produit sur le marché du client_x000D_
+* Et d'autres types de contenu en fonction de votre métier.  _x000D_
+_x000D_
+TalktoB vous propose d'automatiser cette seconde partie, afin que vos collaborateurs n'aient plus d'autres soucis que la satisfaction de client et la conquête de nouveaux **leads**. _x000D_
+_x000D_
+**Le principe** : À partir de vos propres documents Word, Talktob injecte des blocs de contenus avec l'ensemble des données IT. Pour vos commerciaux tout est simplifié, en allant sur la page d'un client il suffira de cliquer sur une offre de son choix et Talktob générera une offre adaptée au client. Votre équipe marketing / communication aura la main sur les templates et pourra modifier les offres à tout moment. _x000D_
+_x000D_
+Outre le gain de temps, la fin des erreurs de copier/coller, vous assurerez aussi une image de marque cohérente sur l'ensemble de vos offres.</t>
+  </si>
+  <si>
+    <t>[{"title":"Injection de donn\u00e9es dans un document Word","id":"390950852","bg":"","_group":"vimeo"}]</t>
+  </si>
+  <si>
+    <t>fideliser-vos-clients</t>
+  </si>
+  <si>
+    <t>repondre-a-un-appel-doffre-public</t>
+  </si>
+  <si>
+    <t>envoyer-des-emails-de-masse-hypercible</t>
+  </si>
+  <si>
+    <t>envoyer-des-emails-de-performance-hebdomadaire</t>
+  </si>
+  <si>
+    <t>En associant nos solutions d'**absorptions**, de **traitement** et de **publication** de données, vous serez en mesure d'envoyer chaque jour des rapports financiers, de suivi, des bilans à vos collaborateurs et clients. _x000D_
+_x000D_
+En utilisant notre système d'email, vous pourrez diffuser chaque jour vos **chiffres** de manière **sécurisée** à un réseau que vous aurez déterminé. _x000D_
+_x000D_
+Notre approche métier étant **100% dédié**, nous serons en mesure de satisfaire toutes vos exigences.</t>
+  </si>
+  <si>
+    <t>[{"carousel_left":"0","show_button":"1","size_text":"w-3\/4","size_carousel":"w-1\/4","title":"Vos KPI au petit d\u00e9jeuner","text":"&lt;p&gt;Il vous sera possible de g\u00e9n\u00e9rer des rapports sur vos chiffres cl\u00e9s.&amp;nbsp;&lt;\/p&gt;\r\n\r\n&lt;p&gt;Vos collaborateurs, vos prestataires et vos clients principaux seront toujours inform\u00e9s !&amp;nbsp;&lt;\/p&gt;\r\n","carousel":[{"text":"Exemple client goose","image":"\/start_images\/phone-chart-cli-srcgoose.png"},{"text":"Exemple client london","image":"\/start_images\/phone_chart-london.png"},{"text":"Exemple client Jungle","image":"\/start_images\/phone-chart-jungle.png"},{"text":"Exemple client Rapid","image":"\/start_images\/phone-chart-rapid.png"}],"_group":"carousel_text"}]</t>
+  </si>
+  <si>
+    <t>bilan-annuel-bu-ou-lead-client</t>
+  </si>
+  <si>
+    <t>publier-de-la-documentation</t>
+  </si>
+  <si>
+    <t>Créer automatiquement des documents</t>
+  </si>
+  <si>
+    <t>controle-dinformation</t>
+  </si>
+  <si>
+    <t>suivi-de-projet</t>
+  </si>
+  <si>
+    <t>Tenez vos clients informés de l'avancement d'un projet</t>
+  </si>
+  <si>
+    <t>Partagez avec vos clients vos documents.  _x000D_
+L'application est capable de se connecter avec vos espaces de stockage cloud:_x000D_
+* One Drive_x000D_
+* Google Drive_x000D_
+* Amazon_x000D_
+* Drop box_x000D_
+Les documents générés par l'application seront ainsi immédiatement disponibles dans vos documents partagés. _x000D_
+_x000D_
+Vous pouvez aussi envoyer vos suivis par email ou afficher l'ensemble des documents que vous souhaitez sur un portail de service client.</t>
+  </si>
+  <si>
+    <t>[{"title":"Trait\u00e9 un projet sur Talktob","text":"&lt;p&gt;Nous n'avons pas de mod\u00e8le pr\u00e9d\u00e9fini, c'est apr\u00e8s une phase d'\u00e9tude sur vos m\u00e9thodes projet que nous vous proposerons l'interface la plus adapt\u00e9e \u00e0 vos besoins.&lt;\/p&gt;\r\n\r\n&lt;p&gt;Nous savons qu'il est souvent difficile de convaincre un client de s'approprier un autre outil, c'est pourquoi il est possible de rendre le syst\u00e8me transparent si le client ne veut pas se connecter sur un portail au moyen de mails et de pi\u00e8ces jointes g\u00e9n\u00e9r\u00e9es automatiquement en PDF ou WORD.&lt;\/p&gt;\r\n","_group":"text"}]</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>main_image</t>
+  </si>
+  <si>
+    <t>montageLinkedin.jpg</t>
+  </si>
+  <si>
+    <t>portail_service.jpg</t>
+  </si>
+  <si>
+    <t>dc1234.jpg</t>
+  </si>
+  <si>
+    <t>campagne_email2.jpg</t>
+  </si>
+  <si>
+    <t>boite_email_gmail.jpg</t>
+  </si>
+  <si>
+    <t>stat_publish.jpg</t>
+  </si>
+  <si>
+    <t>stats_email.jpg</t>
+  </si>
+  <si>
+    <t>crm_survey.jpg</t>
+  </si>
+  <si>
+    <t>avancement_projet.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,17 +289,36 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -248,30 +347,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{DC440D50-6D59-4B41-B898-EDBE8D25AA91}"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -289,6 +406,7 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -363,15 +481,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{316CB12F-A1F8-4323-8D5B-247DC6B6657A}" name="Tableau1" displayName="Tableau1" ref="A1:G10" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5">
-  <autoFilter ref="A1:G10" xr:uid="{6C318A8B-944D-445D-95E0-9D1444D32BE3}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{316CB12F-A1F8-4323-8D5B-247DC6B6657A}" name="Tableau1" displayName="Tableau1" ref="A1:I10" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:I10" xr:uid="{6C318A8B-944D-445D-95E0-9D1444D32BE3}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{496A52CA-7716-43D5-96DC-35FB83C90D97}" name="name"/>
-    <tableColumn id="2" xr3:uid="{1207D03D-6BA7-4143-BC11-7AD7DCE018B1}" name="main_image"/>
+    <tableColumn id="9" xr3:uid="{BE0604EE-56D7-46DC-88F6-166D12C69ABA}" name="main_image" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{1207D03D-6BA7-4143-BC11-7AD7DCE018B1}" name="slug"/>
     <tableColumn id="3" xr3:uid="{5C04322D-21D0-44C6-82D9-47692CE201C3}" name="intro"/>
     <tableColumn id="4" xr3:uid="{5F53B788-34AA-433D-8A1B-61712DC094DD}" name="catchline" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{CC45F14A-9DD9-44AC-8929-C4FC9FD94C2E}" name="description" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{3F6A5929-9C01-4247-A491-AAA4C4173147}" name="kpi" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{71F2CEA6-8E40-4E72-9DD4-70B20CBBB5A0}" name="content"/>
+    <tableColumn id="6" xr3:uid="{3F6A5929-9C01-4247-A491-AAA4C4173147}" name="solutions" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{A1081CD8-9302-49BD-8E75-17339BCB53D6}" name="icone" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -675,199 +795,270 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF79DB02-0089-4E5A-9F1C-E614A24F3FCC}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.9296875" customWidth="1"/>
-    <col min="2" max="2" width="20.53125" customWidth="1"/>
-    <col min="3" max="3" width="29.3984375" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="1"/>
-    <col min="5" max="5" width="65.73046875" style="1" customWidth="1"/>
-    <col min="6" max="7" width="10.6640625" style="1"/>
+    <col min="1" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.53125" customWidth="1"/>
+    <col min="4" max="4" width="29.3984375" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="1"/>
+    <col min="6" max="6" width="33.06640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="57.3984375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.59765625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>5</v>
       </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="166.5" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>40</v>
-      </c>
+    <row r="8" spans="1:9" s="8" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="6"/>
     </row>
-    <row r="3" spans="1:7" ht="229.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+    <row r="9" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="280.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" ht="178.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" ht="165.75" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="242.25" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="280.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" ht="127.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="10" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="191.25" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="I10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Iversion du seed solution et need
</commit_message>
<xml_diff>
--- a/updates/excels/start_needs.xlsx
+++ b/updates/excels/start_needs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\talktob\plugins\waka\wcms\updates\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A436F1A-1A96-4606-A7C1-40213869BF88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD6CB2D-FFDD-47EA-9D82-B01168C74514}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{39C5C7BC-0F20-4ABA-B1CF-FB175B7B3F19}"/>
   </bookViews>
@@ -77,44 +77,6 @@
     <t>Controlez votre CRM et tenez informez vos collaborateurs</t>
   </si>
   <si>
-    <t>orem ipsum dolor sit amet, consectetur adipiscing elit. Morbi cursus sit amet nulla at egestas. **Integer** eget elit mauris.  
-Proin tristique porta efficitur. Suspendisse potenti. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia Curae; Aliquam semper, ante ut bibendum cursus, tellus urna scelerisque sem, ac viverra tortor tortor nec **libero**.  
-Suspendisse sit amet mauris at augue vestibulum imperdiet id ac tortor. Morbi ac ante euismod, consequat quam vitae, volutpat nisi. Nam aliquet aliquam mi, ut ullamcorper nunc blandit sit amet. Sed ac mattis elit.  
-Integer vestibulum urna at ullamcorper faucibus. Curabitur volutpat justo dui, in mattis est posuere ut. Proin magna sapien, posuere ut dignissim fringilla, ultricies at felis. Aliquam suscipit faucibus magna, ac egestas quam scelerisque id. Sed libero nisi, semper ac ipsum non, eleifend facilisis justo
-  * salut
-  * toi
-  * 
-Pellentesque viverra metus in erat semper bibendum. Vivamus auctor venenatis magna eget fermentum.</t>
-  </si>
-  <si>
-    <t>orem ipsum dolor sit amet, consectetur adipiscing elit. Morbi cursus sit amet nulla at egestas. **Integer** eget elit mauris.  
-Proin tristique porta efficitur. Suspendisse potenti. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posue     
-Integer vestibulum urna at ullamcorper faucibus. Curabitur volutpat justo dui, in mattis est posuere ut. Proin magna sapien, posuere ut dignissim fringilla, ultricies at felis. Aliquam suscipit faucibus magna, ac egestas quam scelerisque id. Sed libero nisi, semper ac ipsum non, eleifend facilisis justo
-  * salut
-  * toi
-  * 
-Pellentesque viverra metus in erat semper bibendum. Vivamus auctor venenatis magna eget fermentum.</t>
-  </si>
-  <si>
-    <t>orem ipsum dolor sit amet, consectetur adipiscing elit. Morbi cursus sit amet nulla at egestas. **Intllus urna scelerisque sem, ac viverra tortor tortor nec **libero**.  
-Suspendisse sit amet mauris at augue vestibulum imperdiet id ac tortor. Morbi ac ante euismod, consequat quam vitae, volutpat nisi. Nam aliquet aliquam mi, ut ullamcorper nunc blandit sit amet. Sed ac mattis elit.  
-Integer vestibulum urna at ullamcorper faucibus. Curabitur volutpat justo dui, in mattis est posuere ut. Proin magna sapien, posuere ut dignissim fringilla, ultricies at felis. Aliquam suscipit faucibus magna, ac egestas quam scelerisque id. Sed libero nisi, semper ac ipsum non, eleifend facilisis justo
-  * salut
-  * toi
-  * 
-Pellentesque viverra metus in erat semper bibendum. Vivamus auctor venenatis magna eget fermentum.</t>
-  </si>
-  <si>
-    <t>orem ipsum dolor sit amet, consectetur adipiscing elit. Morbi cursus sit amet nulla at egestas. **Integer** eget elit mauris.  
-Proin tristique porta efficitur. Suspendisse potenti. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia Curae; Aliquam semper, ante ut bibendum cursus, tellus urna scelerisque sem, ac viverra tortor tortor nec **libero**.  
-   Pellentesque viverra metus in erat semper bibendum. Vivamus auctor venenatis magna eget fermentum.</t>
-  </si>
-  <si>
-    <t>Pourquoi fideliser : 
-* A court terme : sur des marchés de plus en plus saturés, où la situation concurrentielle se durcit, il apparait que les coûts de prospection de nouveaux clients sont supérieurs aux couts de conservation des clients. Dans cette hypothèse, un opérateur rationnel préfère investir pour conserver les clients qu'il a, plutôt que de tenter de conquérir les clients servis par d'autres fournisseurs. Lesquels en général ne se laisseront pas faire et feront tout pour conserver leurs clients et en particulier les meilleurs. D'où le risque probable de déclenchement d'une guerre des prix, débouchant à terme sur des effets quasi nuls, sinon négatifs : Le partage des volumes reste peu ou prou identique, tandis que le marché global accuse une baisse générale des prix.
-* A moyen, long terme : les études montrent qu'il existe - en longue période - une corrélation entre capacité d'une organisation à fidéliser ses clients (Taux de rétention élevé) et ses résultats concrets (exprimés en part de marché, en rentabilité et en croissance). Les entreprises qui sont en mesure de conserver leur base clientèle et en particulier leurs « bons clients » sont celles qui non seulement résistent le mieux aux dépressions conjoncturelles, mais aussi sont les plus capables de financer leurs projets de développement.</t>
-  </si>
-  <si>
     <t>solutions</t>
   </si>
   <si>
@@ -170,19 +132,6 @@
   </si>
   <si>
     <t>faire-une-offre</t>
-  </si>
-  <si>
-    <t>Dans une offre, il y a le coeur de votre proposition, celle où le commercial traduit la problématique du prospect et prouve le bénéfice qu'amènera votre produit ou votre solution. Il y a aussi des contenus qui vont renforcer l'argumentaire : _x000D_
-* Des études de cas client_x000D_
-* Des références_x000D_
-* Le positionnement de votre marque/produit sur le marché du client_x000D_
-* Et d'autres types de contenu en fonction de votre métier.  _x000D_
-_x000D_
-TalktoB vous propose d'automatiser cette seconde partie, afin que vos collaborateurs n'aient plus d'autres soucis que la satisfaction de client et la conquête de nouveaux **leads**. _x000D_
-_x000D_
-**Le principe** : À partir de vos propres documents Word, Talktob injecte des blocs de contenus avec l'ensemble des données IT. Pour vos commerciaux tout est simplifié, en allant sur la page d'un client il suffira de cliquer sur une offre de son choix et Talktob générera une offre adaptée au client. Votre équipe marketing / communication aura la main sur les templates et pourra modifier les offres à tout moment. _x000D_
-_x000D_
-Outre le gain de temps, la fin des erreurs de copier/coller, vous assurerez aussi une image de marque cohérente sur l'ensemble de vos offres.</t>
   </si>
   <si>
     <t>[{"title":"Injection de donn\u00e9es dans un document Word","id":"390950852","bg":"","_group":"vimeo"}]</t>
@@ -273,6 +222,65 @@
   </si>
   <si>
     <t>avancement_projet.jpg</t>
+  </si>
+  <si>
+    <t>Pourquoi fideliser : _x000D_
+* A court terme : sur des marchés de plus en plus saturés, où la situation concurrentielle se durcit, il apparait que les coûts de prospection de nouveaux clients sont supérieurs aux couts de conservation des clients. Dans cette hypothèse, un opérateur rationnel préfère investir pour conserver les clients qu'il a, plutôt que de tenter de conquérir les clients servis par d'autres fournisseurs. Lesquels en général ne se laisseront pas faire et feront tout pour conserver leurs clients et en particulier les meilleurs. D'où le risque probable de déclenchement d'une guerre des prix, débouchant à terme sur des effets quasi nuls, sinon négatifs : Le partage des volumes reste peu ou prou identique, tandis que le marché global accuse une baisse générale des prix._x000D_
+* A moyen, long terme : les études montrent qu'il existe - en longue période - une corrélation entre capacité d'une organisation à fidéliser ses clients (Taux de rétention élevé) et ses résultats concrets (exprimés en part de marché, en rentabilité et en croissance). Les entreprises qui sont en mesure de conserver leur base clientèle et en particulier leurs « bons clients » sont celles qui non seulement résistent le mieux aux dépressions conjoncturelles, mais aussi sont les plus capables de financer leurs projets de développement.</t>
+  </si>
+  <si>
+    <t>orem ipsum dolor sit amet, consectetur adipiscing elit. Morbi cursus sit amet nulla at egestas. **Integer** eget elit mauris.  _x000D_
+Proin tristique porta efficitur. Suspendisse potenti. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia Curae; Aliquam semper, ante ut bibendum cursus, tellus urna scelerisque sem, ac viverra tortor tortor nec **libero**.  _x000D_
+   _x000D_
+   _x000D_
+Suspendisse sit amet mauris at augue vestibulum imperdiet id ac tortor. Morbi ac ante euismod, consequat quam vitae, volutpat nisi. Nam aliquet aliquam mi, ut ullamcorper nunc blandit sit amet. Sed ac mattis elit.  _x000D_
+     _x000D_
+   _x000D_
+Integer vestibulum urna at ullamcorper faucibus. Curabitur volutpat justo dui, in mattis est posuere ut. Proin magna sapien, posuere ut dignissim fringilla, ultricies at felis. Aliquam suscipit faucibus magna, ac egestas quam scelerisque id. Sed libero nisi, semper ac ipsum non, eleifend facilisis justo_x000D_
+  * salut_x000D_
+  * toi_x000D_
+  * _x000D_
+Pellentesque viverra metus in erat semper bibendum. Vivamus auctor venenatis magna eget fermentum.</t>
+  </si>
+  <si>
+    <t>orem ipsum dolor sit amet, consectetur adipiscing elit. Morbi cursus sit amet nulla at egestas. **Integer** eget elit mauris.  _x000D_
+Proin tristique porta efficitur. Suspendisse potenti. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posue     _x000D_
+   _x000D_
+Integer vestibulum urna at ullamcorper faucibus. Curabitur volutpat justo dui, in mattis est posuere ut. Proin magna sapien, posuere ut dignissim fringilla, ultricies at felis. Aliquam suscipit faucibus magna, ac egestas quam scelerisque id. Sed libero nisi, semper ac ipsum non, eleifend facilisis justo_x000D_
+  * salut_x000D_
+  * toi_x000D_
+  * _x000D_
+Pellentesque viverra metus in erat semper bibendum. Vivamus auctor venenatis magna eget fermentum.</t>
+  </si>
+  <si>
+    <t>orem ipsum dolor sit amet, consectetur adipiscing elit. Morbi cursus sit amet nulla at egestas. **Intllus urna scelerisque sem, ac viverra tortor tortor nec **libero**.  _x000D_
+   _x000D_
+   _x000D_
+Suspendisse sit amet mauris at augue vestibulum imperdiet id ac tortor. Morbi ac ante euismod, consequat quam vitae, volutpat nisi. Nam aliquet aliquam mi, ut ullamcorper nunc blandit sit amet. Sed ac mattis elit.  _x000D_
+     _x000D_
+   _x000D_
+Integer vestibulum urna at ullamcorper faucibus. Curabitur volutpat justo dui, in mattis est posuere ut. Proin magna sapien, posuere ut dignissim fringilla, ultricies at felis. Aliquam suscipit faucibus magna, ac egestas quam scelerisque id. Sed libero nisi, semper ac ipsum non, eleifend facilisis justo_x000D_
+  * salut_x000D_
+  * toi_x000D_
+  * _x000D_
+Pellentesque viverra metus in erat semper bibendum. Vivamus auctor venenatis magna eget fermentum.</t>
+  </si>
+  <si>
+    <t>orem ipsum dolor sit amet, consectetur adipiscing elit. Morbi cursus sit amet nulla at egestas. **Integer** eget elit mauris.  _x000D_
+Proin tristique porta efficitur. Suspendisse potenti. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia Curae; Aliquam semper, ante ut bibendum cursus, tellus urna scelerisque sem, ac viverra tortor tortor nec **libero**.  _x000D_
+   _x000D_
+     _x000D_
+   Pellentesque viverra metus in erat semper bibendum. Vivamus auctor venenatis magna eget fermentum.</t>
+  </si>
+  <si>
+    <t>Dans une offre, il y a le coeur de votre proposition, celle où le commercial traduit la problématique du prospect et prouve le bénéfice qu'amènera votre produit ou votre solution. Il y a aussi des contenus qui vont renforcer l'argumentaire : 
+* Des études de cas client
+* Des références
+* Le positionnement de votre marque/produit sur le marché du client
+* Et d'autres types de contenu en fonction de votre métier.  
+TalktoB vous propose d'automatiser cette seconde partie, afin que vos collaborateurs n'aient plus d'autres soucis que la satisfaction de client et la conquête de nouveaux **leads**. 
+**Le principe** : À partir de vos propres documents Word, Talktob injecte des blocs de contenus avec l'ensemble des données IT. Pour vos commerciaux tout est simplifié, en allant sur la page d'un client il suffira de cliquer sur une offre de son choix et Talktob générera une offre adaptée au client. Votre équipe marketing / communication aura la main sur les templates et pourra modifier les offres à tout moment. 
+Outre le gain de temps, la fin des erreurs de copier/coller, vous assurerez aussi une image de marque cohérente sur l'ensemble de vos offres.</t>
   </si>
 </sst>
 </file>
@@ -351,7 +359,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -385,29 +393,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{DC440D50-6D59-4B41-B898-EDBE8D25AA91}"/>
   </cellStyles>
   <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -425,6 +419,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.79998168889431442"/>
@@ -432,7 +427,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
         <top style="thin">
@@ -442,6 +437,23 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -489,10 +501,10 @@
     <tableColumn id="2" xr3:uid="{1207D03D-6BA7-4143-BC11-7AD7DCE018B1}" name="slug"/>
     <tableColumn id="3" xr3:uid="{5C04322D-21D0-44C6-82D9-47692CE201C3}" name="intro"/>
     <tableColumn id="4" xr3:uid="{5F53B788-34AA-433D-8A1B-61712DC094DD}" name="catchline" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{CC45F14A-9DD9-44AC-8929-C4FC9FD94C2E}" name="description" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{CC45F14A-9DD9-44AC-8929-C4FC9FD94C2E}" name="description" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{71F2CEA6-8E40-4E72-9DD4-70B20CBBB5A0}" name="content"/>
-    <tableColumn id="6" xr3:uid="{3F6A5929-9C01-4247-A491-AAA4C4173147}" name="solutions" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{A1081CD8-9302-49BD-8E75-17339BCB53D6}" name="icone" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{3F6A5929-9C01-4247-A491-AAA4C4173147}" name="solutions" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{A1081CD8-9302-49BD-8E75-17339BCB53D6}" name="icone" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -797,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF79DB02-0089-4E5A-9F1C-E614A24F3FCC}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -807,7 +819,7 @@
     <col min="3" max="3" width="20.53125" customWidth="1"/>
     <col min="4" max="4" width="29.3984375" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" style="1"/>
-    <col min="6" max="6" width="33.06640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="77.796875" style="1" customWidth="1"/>
     <col min="7" max="7" width="57.3984375" style="1" customWidth="1"/>
     <col min="8" max="8" width="21.59765625" style="1" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" style="1"/>
@@ -818,10 +830,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -833,10 +845,10 @@
         <v>3</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -844,165 +856,165 @@
     </row>
     <row r="2" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="9"/>
-      <c r="F2" s="9" t="s">
-        <v>38</v>
+      <c r="F2" s="15" t="s">
+        <v>64</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="9"/>
-      <c r="F3" s="9" t="s">
-        <v>18</v>
+      <c r="F3" s="15" t="s">
+        <v>59</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="9"/>
-      <c r="F4" s="9" t="s">
-        <v>14</v>
+      <c r="F4" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="9"/>
-      <c r="F5" s="9" t="s">
-        <v>15</v>
+      <c r="F5" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="9"/>
-      <c r="F6" s="9" t="s">
-        <v>44</v>
+      <c r="F6" s="15" t="s">
+        <v>38</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="9"/>
-      <c r="F7" s="9" t="s">
-        <v>16</v>
+      <c r="F7" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" s="8" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E8" s="9"/>
-      <c r="F8" s="9" t="s">
-        <v>14</v>
+      <c r="F8" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I8" s="6"/>
     </row>
@@ -1011,21 +1023,21 @@
         <v>7</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="9"/>
-      <c r="F9" s="9" t="s">
-        <v>17</v>
+      <c r="F9" s="15" t="s">
+        <v>63</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I9" s="2"/>
     </row>
@@ -1034,23 +1046,23 @@
         <v>8</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E10" s="9"/>
-      <c r="F10" s="9" t="s">
-        <v>52</v>
+      <c r="F10" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I10" s="2"/>
     </row>

</xml_diff>

<commit_message>
ajout state aux pages
</commit_message>
<xml_diff>
--- a/updates/excels/start_needs.xlsx
+++ b/updates/excels/start_needs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\talktob\plugins\waka\wcms\updates\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD6CB2D-FFDD-47EA-9D82-B01168C74514}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F535C7-8C5E-4655-93A8-CFD312689206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{39C5C7BC-0F20-4ABA-B1CF-FB175B7B3F19}"/>
   </bookViews>
@@ -149,13 +149,6 @@
     <t>envoyer-des-emails-de-performance-hebdomadaire</t>
   </si>
   <si>
-    <t>En associant nos solutions d'**absorptions**, de **traitement** et de **publication** de données, vous serez en mesure d'envoyer chaque jour des rapports financiers, de suivi, des bilans à vos collaborateurs et clients. _x000D_
-_x000D_
-En utilisant notre système d'email, vous pourrez diffuser chaque jour vos **chiffres** de manière **sécurisée** à un réseau que vous aurez déterminé. _x000D_
-_x000D_
-Notre approche métier étant **100% dédié**, nous serons en mesure de satisfaire toutes vos exigences.</t>
-  </si>
-  <si>
     <t>[{"carousel_left":"0","show_button":"1","size_text":"w-3\/4","size_carousel":"w-1\/4","title":"Vos KPI au petit d\u00e9jeuner","text":"&lt;p&gt;Il vous sera possible de g\u00e9n\u00e9rer des rapports sur vos chiffres cl\u00e9s.&amp;nbsp;&lt;\/p&gt;\r\n\r\n&lt;p&gt;Vos collaborateurs, vos prestataires et vos clients principaux seront toujours inform\u00e9s !&amp;nbsp;&lt;\/p&gt;\r\n","carousel":[{"text":"Exemple client goose","image":"\/start_images\/phone-chart-cli-srcgoose.png"},{"text":"Exemple client london","image":"\/start_images\/phone_chart-london.png"},{"text":"Exemple client Jungle","image":"\/start_images\/phone-chart-jungle.png"},{"text":"Exemple client Rapid","image":"\/start_images\/phone-chart-rapid.png"}],"_group":"carousel_text"}]</t>
   </si>
   <si>
@@ -175,17 +168,6 @@
   </si>
   <si>
     <t>Tenez vos clients informés de l'avancement d'un projet</t>
-  </si>
-  <si>
-    <t>Partagez avec vos clients vos documents.  _x000D_
-L'application est capable de se connecter avec vos espaces de stockage cloud:_x000D_
-* One Drive_x000D_
-* Google Drive_x000D_
-* Amazon_x000D_
-* Drop box_x000D_
-Les documents générés par l'application seront ainsi immédiatement disponibles dans vos documents partagés. _x000D_
-_x000D_
-Vous pouvez aussi envoyer vos suivis par email ou afficher l'ensemble des documents que vous souhaitez sur un portail de service client.</t>
   </si>
   <si>
     <t>[{"title":"Trait\u00e9 un projet sur Talktob","text":"&lt;p&gt;Nous n'avons pas de mod\u00e8le pr\u00e9d\u00e9fini, c'est apr\u00e8s une phase d'\u00e9tude sur vos m\u00e9thodes projet que nous vous proposerons l'interface la plus adapt\u00e9e \u00e0 vos besoins.&lt;\/p&gt;\r\n\r\n&lt;p&gt;Nous savons qu'il est souvent difficile de convaincre un client de s'approprier un autre outil, c'est pourquoi il est possible de rendre le syst\u00e8me transparent si le client ne veut pas se connecter sur un portail au moyen de mails et de pi\u00e8ces jointes g\u00e9n\u00e9r\u00e9es automatiquement en PDF ou WORD.&lt;\/p&gt;\r\n","_group":"text"}]</t>
@@ -281,6 +263,21 @@
 TalktoB vous propose d'automatiser cette seconde partie, afin que vos collaborateurs n'aient plus d'autres soucis que la satisfaction de client et la conquête de nouveaux **leads**. 
 **Le principe** : À partir de vos propres documents Word, Talktob injecte des blocs de contenus avec l'ensemble des données IT. Pour vos commerciaux tout est simplifié, en allant sur la page d'un client il suffira de cliquer sur une offre de son choix et Talktob générera une offre adaptée au client. Votre équipe marketing / communication aura la main sur les templates et pourra modifier les offres à tout moment. 
 Outre le gain de temps, la fin des erreurs de copier/coller, vous assurerez aussi une image de marque cohérente sur l'ensemble de vos offres.</t>
+  </si>
+  <si>
+    <t>En associant nos solutions d'**absorptions**, de **traitement** et de **publication** de données, vous serez en mesure d'envoyer chaque jour des rapports financiers, de suivi, des bilans à vos collaborateurs et clients.  
+En utilisant notre système d'email, vous pourrez diffuser chaque jour vos **chiffres** de manière **sécurisée** à un réseau que vous aurez déterminé.  
+Notre approche métier étant **100% dédié**, nous serons en mesure de satisfaire toutes vos exigences.</t>
+  </si>
+  <si>
+    <t>Partagez avec vos clients vos documents.  
+L'application est capable de se connecter avec vos espaces de stockage cloud:
+* One Drive
+* Google Drive
+* Amazon
+* Drop box
+Les documents générés par l'application seront ainsi immédiatement disponibles dans vos documents partagés. 
+Vous pouvez aussi envoyer vos suivis par email ou afficher l'ensemble des documents que vous souhaitez sur un portail de service client.</t>
   </si>
 </sst>
 </file>
@@ -403,6 +400,23 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -437,23 +451,6 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -501,10 +498,10 @@
     <tableColumn id="2" xr3:uid="{1207D03D-6BA7-4143-BC11-7AD7DCE018B1}" name="slug"/>
     <tableColumn id="3" xr3:uid="{5C04322D-21D0-44C6-82D9-47692CE201C3}" name="intro"/>
     <tableColumn id="4" xr3:uid="{5F53B788-34AA-433D-8A1B-61712DC094DD}" name="catchline" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{CC45F14A-9DD9-44AC-8929-C4FC9FD94C2E}" name="description" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{CC45F14A-9DD9-44AC-8929-C4FC9FD94C2E}" name="description" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{71F2CEA6-8E40-4E72-9DD4-70B20CBBB5A0}" name="content"/>
-    <tableColumn id="6" xr3:uid="{3F6A5929-9C01-4247-A491-AAA4C4173147}" name="solutions" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{A1081CD8-9302-49BD-8E75-17339BCB53D6}" name="icone" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{3F6A5929-9C01-4247-A491-AAA4C4173147}" name="solutions" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{A1081CD8-9302-49BD-8E75-17339BCB53D6}" name="icone" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -809,15 +806,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF79DB02-0089-4E5A-9F1C-E614A24F3FCC}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="2" width="33.33203125" customWidth="1"/>
     <col min="3" max="3" width="20.53125" customWidth="1"/>
-    <col min="4" max="4" width="29.3984375" customWidth="1"/>
+    <col min="4" max="4" width="46.06640625" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" style="1"/>
     <col min="6" max="6" width="77.796875" style="1" customWidth="1"/>
     <col min="7" max="7" width="57.3984375" style="1" customWidth="1"/>
@@ -830,7 +827,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>30</v>
@@ -845,7 +842,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>14</v>
@@ -859,7 +856,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>32</v>
@@ -869,7 +866,7 @@
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>33</v>
@@ -883,7 +880,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>34</v>
@@ -893,7 +890,7 @@
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="4" t="s">
@@ -906,7 +903,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>35</v>
@@ -916,7 +913,7 @@
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="4" t="s">
@@ -929,7 +926,7 @@
         <v>24</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>36</v>
@@ -939,7 +936,7 @@
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="5" t="s">
@@ -952,7 +949,7 @@
         <v>25</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>37</v>
@@ -962,10 +959,10 @@
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>39</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>21</v>
@@ -977,17 +974,17 @@
         <v>22</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="4" t="s">
@@ -1000,17 +997,17 @@
         <v>28</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>41</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>42</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="7" t="s">
@@ -1023,17 +1020,17 @@
         <v>7</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="4" t="s">
@@ -1046,20 +1043,20 @@
         <v>8</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>45</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="15" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>27</v>

</xml_diff>